<commit_message>
Added bang-bang control function to slave solution.
</commit_message>
<xml_diff>
--- a/Documentation/Raw_Sensor_Value_Ranges.xlsx
+++ b/Documentation/Raw_Sensor_Value_Ranges.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Coursework\MSME\Thesis\AARL_Puppy_18_00_000\Electronics\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\Quadruped_Robot\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585EBB0A-D29B-43DC-8DF1-6EE10909E263}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34E93423-30B8-4535-B556-CB111EE91520}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{765975E2-55C5-4756-8ED3-1B702E7309E7}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -456,7 +457,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>